<commit_message>
Added data from crunchy 3
</commit_message>
<xml_diff>
--- a/Aggregate Output.xlsx
+++ b/Aggregate Output.xlsx
@@ -47,9 +47,6 @@
     <t>Trial 5</t>
   </si>
   <si>
-    <t>CIMS Crunchy1 Timings</t>
-  </si>
-  <si>
     <t>Speedup</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>N = 10000</t>
+  </si>
+  <si>
+    <t>CIMS Crunchy5 Timings</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -290,6 +290,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,25 +465,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0001278</c:v>
+                  <c:v>0.020622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0005598</c:v>
+                  <c:v>0.0009092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0014516</c:v>
+                  <c:v>0.0020488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0032014</c:v>
+                  <c:v>0.0031892</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0034016</c:v>
+                  <c:v>0.010063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.07382712</c:v>
+                  <c:v>0.0917616</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0785218</c:v>
+                  <c:v>0.0878806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,25 +564,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0009386</c:v>
+                  <c:v>0.0437624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0038754</c:v>
+                  <c:v>0.0056524</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0059068</c:v>
+                  <c:v>0.009627</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0083766</c:v>
+                  <c:v>0.0156058</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0222214</c:v>
+                  <c:v>0.0383302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.07672496</c:v>
+                  <c:v>0.4548478</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.525321</c:v>
+                  <c:v>0.5958638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,11 +598,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2138902704"/>
-        <c:axId val="-2138909920"/>
+        <c:axId val="-2146547456"/>
+        <c:axId val="-2146540416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138902704"/>
+        <c:axId val="-2146547456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138909920"/>
+        <c:crossAx val="-2146540416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -705,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138909920"/>
+        <c:axId val="-2146540416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138902704"/>
+        <c:crossAx val="-2146547456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1052,22 +1056,22 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.228295819935691</c:v>
+                  <c:v>22.68147822261329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0880407825847341</c:v>
+                  <c:v>10.0654041390082</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0399200349846942</c:v>
+                  <c:v>6.466198419666373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0375705550329257</c:v>
+                  <c:v>2.049289476299315</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00173107118359757</c:v>
+                  <c:v>0.224734529476382</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00162757348914569</c:v>
+                  <c:v>0.234659299094453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1151,22 +1155,22 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.242194354131186</c:v>
+                  <c:v>7.74226877078763</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.158901604929911</c:v>
+                  <c:v>4.545798275682974</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.112050235178951</c:v>
+                  <c:v>2.804239449435467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0422385628268246</c:v>
+                  <c:v>1.141721149380906</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0122333071271722</c:v>
+                  <c:v>0.0962132827728308</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00178671707394146</c:v>
+                  <c:v>0.0734436292320493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,11 +1186,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2138991376"/>
-        <c:axId val="-2138997200"/>
+        <c:axId val="-2147327760"/>
+        <c:axId val="-2147333584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138991376"/>
+        <c:axId val="-2147327760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +1293,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138997200"/>
+        <c:crossAx val="-2147333584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1297,7 +1301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138997200"/>
+        <c:axId val="-2147333584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138991376"/>
+        <c:crossAx val="-2147327760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1642,25 +1646,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7824.726134585288</c:v>
+                  <c:v>48.49190185239065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1786.352268667381</c:v>
+                  <c:v>1099.868015838099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>688.8950124001102</c:v>
+                  <c:v>488.0905896134322</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>312.3633410382957</c:v>
+                  <c:v>313.5582591245452</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>293.9793038570085</c:v>
+                  <c:v>99.37394415184339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.54515793112341</c:v>
+                  <c:v>10.89780474621192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.73531681647644</c:v>
+                  <c:v>11.379075700439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1741,25 +1745,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1065.416577881952</c:v>
+                  <c:v>22.85066632543005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>258.0378799607782</c:v>
+                  <c:v>176.9160002830656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169.296404144376</c:v>
+                  <c:v>103.8745195803469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119.3801781152257</c:v>
+                  <c:v>64.07873995565751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.00166506160728</c:v>
+                  <c:v>26.08908902118956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.03356821561067</c:v>
+                  <c:v>2.198537620716204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.903597990561961</c:v>
+                  <c:v>1.67823586531016</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1775,11 +1779,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2139041984"/>
-        <c:axId val="-2139047808"/>
+        <c:axId val="-2147378368"/>
+        <c:axId val="-2147384192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2139041984"/>
+        <c:axId val="-2147378368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2139047808"/>
+        <c:crossAx val="-2147384192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1890,7 +1894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139047808"/>
+        <c:axId val="-2147384192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +2000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2139041984"/>
+        <c:crossAx val="-2147378368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2234,25 +2238,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0001278</c:v>
+                  <c:v>0.020622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0005598</c:v>
+                  <c:v>0.0009092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0014516</c:v>
+                  <c:v>0.0020488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0032014</c:v>
+                  <c:v>0.0031892</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0034016</c:v>
+                  <c:v>0.010063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.07382712</c:v>
+                  <c:v>0.0917616</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0785218</c:v>
+                  <c:v>0.0878806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,11 +2272,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2089147040"/>
-        <c:axId val="-2133435216"/>
+        <c:axId val="-2147417584"/>
+        <c:axId val="-2147423344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2089147040"/>
+        <c:axId val="-2147417584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2375,7 +2379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133435216"/>
+        <c:crossAx val="-2147423344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2383,7 +2387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133435216"/>
+        <c:axId val="-2147423344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089147040"/>
+        <c:crossAx val="-2147417584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2725,25 +2729,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0009386</c:v>
+                  <c:v>0.0437624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0038754</c:v>
+                  <c:v>0.0056524</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0059068</c:v>
+                  <c:v>0.009627</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0083766</c:v>
+                  <c:v>0.0156058</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0222214</c:v>
+                  <c:v>0.0383302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.07672496</c:v>
+                  <c:v>0.4548478</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.525321</c:v>
+                  <c:v>0.5958638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2759,11 +2763,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2095359936"/>
-        <c:axId val="-2093039744"/>
+        <c:axId val="-2147458992"/>
+        <c:axId val="-2147464752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095359936"/>
+        <c:axId val="-2147458992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2867,7 +2871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093039744"/>
+        <c:crossAx val="-2147464752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2875,7 +2879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093039744"/>
+        <c:axId val="-2147464752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2981,7 +2985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095359936"/>
+        <c:crossAx val="-2147458992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3190,22 +3194,22 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.228295819935691</c:v>
+                  <c:v>22.68147822261329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0880407825847341</c:v>
+                  <c:v>10.0654041390082</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0399200349846942</c:v>
+                  <c:v>6.466198419666373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0375705550329257</c:v>
+                  <c:v>2.049289476299315</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00173107118359757</c:v>
+                  <c:v>0.224734529476382</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00162757348914569</c:v>
+                  <c:v>0.234659299094453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3221,11 +3225,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2085663744"/>
-        <c:axId val="-2129690608"/>
+        <c:axId val="-2143034576"/>
+        <c:axId val="-2143029024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2085663744"/>
+        <c:axId val="-2143034576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,7 +3328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129690608"/>
+        <c:crossAx val="-2143029024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3332,7 +3336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129690608"/>
+        <c:axId val="-2143029024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3439,7 +3443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085663744"/>
+        <c:crossAx val="-2143034576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3648,22 +3652,22 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.242194354131186</c:v>
+                  <c:v>7.74226877078763</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.158901604929911</c:v>
+                  <c:v>4.545798275682974</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.112050235178951</c:v>
+                  <c:v>2.804239449435467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0422385628268246</c:v>
+                  <c:v>1.141721149380906</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0122333071271722</c:v>
+                  <c:v>0.0962132827728308</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00178671707394146</c:v>
+                  <c:v>0.0734436292320493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3679,11 +3683,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2086803936"/>
-        <c:axId val="-2133220352"/>
+        <c:axId val="-2142994432"/>
+        <c:axId val="-2142988688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2086803936"/>
+        <c:axId val="-2142994432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,7 +3790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133220352"/>
+        <c:crossAx val="-2142988688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3794,7 +3798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133220352"/>
+        <c:axId val="-2142988688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3900,7 +3904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086803936"/>
+        <c:crossAx val="-2142994432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4106,25 +4110,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7824.726134585288</c:v>
+                  <c:v>48.49190185239065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1786.352268667381</c:v>
+                  <c:v>1099.868015838099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>688.8950124001102</c:v>
+                  <c:v>488.0905896134322</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>312.3633410382957</c:v>
+                  <c:v>313.5582591245452</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>293.9793038570085</c:v>
+                  <c:v>99.37394415184339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.54515793112341</c:v>
+                  <c:v>10.89780474621192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.73531681647644</c:v>
+                  <c:v>11.379075700439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4140,11 +4144,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2095398512"/>
-        <c:axId val="-2091041920"/>
+        <c:axId val="-2142954176"/>
+        <c:axId val="-2142948432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095398512"/>
+        <c:axId val="-2142954176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4248,7 +4252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091041920"/>
+        <c:crossAx val="-2142948432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4256,7 +4260,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091041920"/>
+        <c:axId val="-2142948432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,7 +4366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095398512"/>
+        <c:crossAx val="-2142954176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4568,25 +4572,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1065.416577881952</c:v>
+                  <c:v>22.85066632543005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>258.0378799607782</c:v>
+                  <c:v>176.9160002830656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169.296404144376</c:v>
+                  <c:v>103.8745195803469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119.3801781152257</c:v>
+                  <c:v>64.07873995565751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.00166506160728</c:v>
+                  <c:v>26.08908902118956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.03356821561067</c:v>
+                  <c:v>2.198537620716204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.903597990561961</c:v>
+                  <c:v>1.67823586531016</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4602,11 +4606,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2088742432"/>
-        <c:axId val="-2054879280"/>
+        <c:axId val="-2142913408"/>
+        <c:axId val="-2142907664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2088742432"/>
+        <c:axId val="-2142913408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4710,7 +4714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054879280"/>
+        <c:crossAx val="-2142907664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4718,7 +4722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054879280"/>
+        <c:axId val="-2142907664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4824,7 +4828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088742432"/>
+        <c:crossAx val="-2142913408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10300,8 +10304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10318,12 +10322,12 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -10346,135 +10350,140 @@
       <c r="H2" s="14">
         <v>100</v>
       </c>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>1.2300000000000001E-4</v>
+        <v>1.9909E-2</v>
       </c>
       <c r="C3" s="16">
-        <v>6.11E-4</v>
+        <v>8.92E-4</v>
       </c>
       <c r="D3" s="16">
-        <v>1.0510000000000001E-3</v>
+        <v>2.029E-3</v>
       </c>
       <c r="E3" s="16">
-        <v>5.5909999999999996E-3</v>
-      </c>
-      <c r="F3" s="16">
-        <v>3.4650000000000002E-3</v>
-      </c>
-      <c r="G3" s="16">
-        <v>7.6444999999999999E-2</v>
-      </c>
-      <c r="H3" s="16">
-        <v>7.8267000000000003E-2</v>
-      </c>
+        <v>2.9220000000000001E-3</v>
+      </c>
+      <c r="F3" s="23">
+        <v>8.7180000000000001E-3</v>
+      </c>
+      <c r="G3" s="23">
+        <v>8.1397999999999998E-2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>8.9732000000000006E-2</v>
+      </c>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="17">
-        <v>1.3200000000000001E-4</v>
+        <v>2.2832999999999999E-2</v>
       </c>
       <c r="C4" s="17">
-        <v>5.3700000000000004E-4</v>
+        <v>9.2299999999999999E-4</v>
       </c>
       <c r="D4" s="17">
-        <v>2.4680000000000001E-3</v>
+        <v>1.7979999999999999E-3</v>
       </c>
       <c r="E4" s="17">
-        <v>1.57E-3</v>
-      </c>
-      <c r="F4" s="17">
-        <v>3.398E-3</v>
-      </c>
-      <c r="G4" s="17">
-        <v>7.3800000000000004E-2</v>
-      </c>
-      <c r="H4" s="17">
-        <v>8.4262000000000004E-2</v>
-      </c>
+        <v>3.3540000000000002E-3</v>
+      </c>
+      <c r="F4" s="24">
+        <v>7.8100000000000001E-3</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0.103229</v>
+      </c>
+      <c r="H4" s="24">
+        <v>9.3645999999999993E-2</v>
+      </c>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="17">
-        <v>1.2999999999999999E-4</v>
+        <v>2.0403000000000001E-2</v>
       </c>
       <c r="C5" s="17">
-        <v>5.3600000000000002E-4</v>
+        <v>8.9099999999999997E-4</v>
       </c>
       <c r="D5" s="17">
-        <v>1.684E-3</v>
+        <v>1.9659999999999999E-3</v>
       </c>
       <c r="E5" s="17">
-        <v>1.702E-3</v>
-      </c>
-      <c r="F5" s="17">
-        <v>3.3479999999999998E-3</v>
-      </c>
-      <c r="G5" s="17">
-        <v>7.7098299999999995E-2</v>
-      </c>
-      <c r="H5" s="17">
-        <v>8.0452999999999997E-2</v>
-      </c>
+        <v>3.4030000000000002E-3</v>
+      </c>
+      <c r="F5" s="24">
+        <v>1.2656000000000001E-2</v>
+      </c>
+      <c r="G5" s="24">
+        <v>8.4739999999999996E-2</v>
+      </c>
+      <c r="H5" s="24">
+        <v>8.6196999999999996E-2</v>
+      </c>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="17">
-        <v>1.25E-4</v>
+        <v>1.9569E-2</v>
       </c>
       <c r="C6" s="17">
-        <v>5.5400000000000002E-4</v>
+        <v>9.3499999999999996E-4</v>
       </c>
       <c r="D6" s="17">
-        <v>9.7900000000000005E-4</v>
+        <v>2.5539999999999998E-3</v>
       </c>
       <c r="E6" s="17">
-        <v>1.586E-3</v>
-      </c>
-      <c r="F6" s="17">
-        <v>3.3270000000000001E-3</v>
-      </c>
-      <c r="G6" s="17">
-        <v>7.0101399999999994E-2</v>
-      </c>
-      <c r="H6" s="17">
-        <v>7.3433999999999999E-2</v>
-      </c>
+        <v>3.1089999999999998E-3</v>
+      </c>
+      <c r="F6" s="24">
+        <v>1.0914E-2</v>
+      </c>
+      <c r="G6" s="24">
+        <v>9.8348000000000005E-2</v>
+      </c>
+      <c r="H6" s="24">
+        <v>8.4612999999999994E-2</v>
+      </c>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="18">
-        <v>1.2899999999999999E-4</v>
+        <v>2.0396000000000001E-2</v>
       </c>
       <c r="C7" s="18">
-        <v>5.6099999999999998E-4</v>
+        <v>9.0499999999999999E-4</v>
       </c>
       <c r="D7" s="18">
-        <v>1.0759999999999999E-3</v>
+        <v>1.897E-3</v>
       </c>
       <c r="E7" s="18">
-        <v>5.5579999999999996E-3</v>
-      </c>
-      <c r="F7" s="18">
-        <v>3.47E-3</v>
-      </c>
-      <c r="G7" s="18">
-        <v>7.1690900000000002E-2</v>
-      </c>
-      <c r="H7" s="18">
-        <v>7.6192999999999997E-2</v>
+        <v>3.1580000000000002E-3</v>
+      </c>
+      <c r="F7" s="25">
+        <v>1.0217E-2</v>
+      </c>
+      <c r="G7" s="25">
+        <v>9.1092999999999993E-2</v>
+      </c>
+      <c r="H7" s="25">
+        <v>8.5214999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -10482,32 +10491,32 @@
         <v>0</v>
       </c>
       <c r="B8" s="19">
-        <f t="shared" ref="B8:H8" si="0">AVERAGE(B3:B7)</f>
-        <v>1.2780000000000002E-4</v>
+        <f>AVERAGE(B3:B7)</f>
+        <v>2.0622000000000001E-2</v>
       </c>
       <c r="C8" s="19">
-        <f t="shared" si="0"/>
-        <v>5.5980000000000005E-4</v>
+        <f t="shared" ref="C8:H8" si="0">AVERAGE(C3:C7)</f>
+        <v>9.0919999999999998E-4</v>
       </c>
       <c r="D8" s="19">
         <f t="shared" si="0"/>
-        <v>1.4515999999999999E-3</v>
+        <v>2.0487999999999999E-3</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="0"/>
-        <v>3.2014000000000001E-3</v>
+        <v>3.1892000000000005E-3</v>
       </c>
       <c r="F8" s="20">
         <f t="shared" si="0"/>
-        <v>3.4015999999999998E-3</v>
+        <v>1.0062999999999999E-2</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" si="0"/>
-        <v>7.3827119999999996E-2</v>
+        <v>9.1761599999999985E-2</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="0"/>
-        <v>7.8521800000000003E-2</v>
+        <v>8.7880600000000003E-2</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="6"/>
@@ -10517,7 +10526,7 @@
     </row>
     <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -10546,25 +10555,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="16">
-        <v>9.6500000000000004E-4</v>
+        <v>4.0913999999999999E-2</v>
       </c>
       <c r="C11" s="16">
-        <v>3.3730000000000001E-3</v>
+        <v>5.8349999999999999E-3</v>
       </c>
       <c r="D11" s="16">
-        <v>5.8869999999999999E-3</v>
+        <v>9.4929999999999997E-3</v>
       </c>
       <c r="E11" s="16">
-        <v>8.4860000000000005E-3</v>
+        <v>1.6452000000000001E-2</v>
       </c>
       <c r="F11" s="16">
-        <v>1.77E-2</v>
+        <v>3.7016E-2</v>
       </c>
       <c r="G11" s="16">
-        <v>9.7015000000000004E-2</v>
+        <v>0.49700699999999998</v>
       </c>
       <c r="H11" s="16">
-        <v>0.51466999999999996</v>
+        <v>0.606186</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -10572,25 +10581,25 @@
         <v>2</v>
       </c>
       <c r="B12" s="17">
-        <v>9.1100000000000003E-4</v>
+        <v>9.2521000000000006E-2</v>
       </c>
       <c r="C12" s="17">
-        <v>4.019E-3</v>
+        <v>6.2300000000000003E-3</v>
       </c>
       <c r="D12" s="17">
-        <v>6.0879999999999997E-3</v>
+        <v>9.691E-3</v>
       </c>
       <c r="E12" s="17">
-        <v>8.1399999999999997E-3</v>
+        <v>1.5387E-2</v>
       </c>
       <c r="F12" s="17">
-        <v>1.8176999999999999E-2</v>
+        <v>4.4470000000000003E-2</v>
       </c>
       <c r="G12" s="17">
-        <v>7.4185799999999996E-2</v>
+        <v>0.462974</v>
       </c>
       <c r="H12" s="17">
-        <v>0.52309700000000003</v>
+        <v>0.59176700000000004</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -10598,25 +10607,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="17">
-        <v>9.2400000000000002E-4</v>
+        <v>1.0557E-2</v>
       </c>
       <c r="C13" s="17">
-        <v>3.9490000000000003E-3</v>
+        <v>5.0549999999999996E-3</v>
       </c>
       <c r="D13" s="17">
-        <v>5.77E-3</v>
+        <v>9.665E-3</v>
       </c>
       <c r="E13" s="17">
-        <v>8.567E-3</v>
+        <v>1.4912E-2</v>
       </c>
       <c r="F13" s="17">
-        <v>1.7981E-2</v>
+        <v>3.5777000000000003E-2</v>
       </c>
       <c r="G13" s="17">
-        <v>4.2624000000000002E-2</v>
+        <v>0.37228699999999998</v>
       </c>
       <c r="H13" s="17">
-        <v>0.52522199999999997</v>
+        <v>0.60081899999999999</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -10624,25 +10633,25 @@
         <v>4</v>
       </c>
       <c r="B14" s="17">
-        <v>9.4200000000000002E-4</v>
+        <v>1.8401000000000001E-2</v>
       </c>
       <c r="C14" s="17">
-        <v>4.0260000000000001E-3</v>
+        <v>5.1130000000000004E-3</v>
       </c>
       <c r="D14" s="17">
-        <v>5.9329999999999999E-3</v>
+        <v>9.4859999999999996E-3</v>
       </c>
       <c r="E14" s="17">
-        <v>8.4469999999999996E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F14" s="17">
-        <v>3.9031000000000003E-2</v>
+        <v>3.288E-2</v>
       </c>
       <c r="G14" s="17">
-        <v>7.8161700000000001E-2</v>
+        <v>0.465339</v>
       </c>
       <c r="H14" s="17">
-        <v>0.56020099999999995</v>
+        <v>0.57344399999999995</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -10650,25 +10659,25 @@
         <v>5</v>
       </c>
       <c r="B15" s="18">
-        <v>9.5100000000000002E-4</v>
+        <v>5.6418999999999997E-2</v>
       </c>
       <c r="C15" s="18">
-        <v>4.0099999999999997E-3</v>
+        <v>6.0289999999999996E-3</v>
       </c>
       <c r="D15" s="18">
-        <v>5.8560000000000001E-3</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="E15" s="18">
-        <v>8.2430000000000003E-3</v>
+        <v>1.5278E-2</v>
       </c>
       <c r="F15" s="18">
-        <v>1.8218000000000002E-2</v>
+        <v>4.1508000000000003E-2</v>
       </c>
       <c r="G15" s="18">
-        <v>9.1638300000000006E-2</v>
+        <v>0.476632</v>
       </c>
       <c r="H15" s="18">
-        <v>0.50341499999999995</v>
+        <v>0.60710299999999995</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -10677,31 +10686,31 @@
       </c>
       <c r="B16" s="19">
         <f t="shared" ref="B16:H16" si="1">AVERAGE(B11:B15)</f>
-        <v>9.3860000000000005E-4</v>
+        <v>4.37624E-2</v>
       </c>
       <c r="C16" s="19">
         <f t="shared" si="1"/>
-        <v>3.8753999999999998E-3</v>
+        <v>5.6524000000000001E-3</v>
       </c>
       <c r="D16" s="19">
         <f t="shared" si="1"/>
-        <v>5.9068000000000002E-3</v>
+        <v>9.6270000000000001E-3</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="1"/>
-        <v>8.3766000000000014E-3</v>
+        <v>1.56058E-2</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="1"/>
-        <v>2.2221399999999999E-2</v>
+        <v>3.8330200000000002E-2</v>
       </c>
       <c r="G16" s="19">
         <f t="shared" si="1"/>
-        <v>7.6724959999999995E-2</v>
+        <v>0.45484780000000002</v>
       </c>
       <c r="H16" s="19">
         <f t="shared" si="1"/>
-        <v>0.52532100000000004</v>
+        <v>0.59586379999999994</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -10735,68 +10744,68 @@
     </row>
     <row r="19" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="21">
-        <f>B8</f>
-        <v>1.2780000000000002E-4</v>
+        <f t="shared" ref="B19:H19" si="2">B8</f>
+        <v>2.0622000000000001E-2</v>
       </c>
       <c r="C19" s="16">
-        <f>C8</f>
-        <v>5.5980000000000005E-4</v>
+        <f t="shared" si="2"/>
+        <v>9.0919999999999998E-4</v>
       </c>
       <c r="D19" s="16">
-        <f>D8</f>
-        <v>1.4515999999999999E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.0487999999999999E-3</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" ref="E19:H19" si="2">E8</f>
-        <v>3.2014000000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.1892000000000005E-3</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="2"/>
-        <v>3.4015999999999998E-3</v>
+        <v>1.0062999999999999E-2</v>
       </c>
       <c r="G19" s="16">
         <f t="shared" si="2"/>
-        <v>7.3827119999999996E-2</v>
+        <v>9.1761599999999985E-2</v>
       </c>
       <c r="H19" s="16">
         <f t="shared" si="2"/>
-        <v>7.8521800000000003E-2</v>
+        <v>8.7880600000000003E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="22">
-        <f>B16</f>
-        <v>9.3860000000000005E-4</v>
+        <f t="shared" ref="B20:H20" si="3">B16</f>
+        <v>4.37624E-2</v>
       </c>
       <c r="C20" s="17">
-        <f>C16</f>
-        <v>3.8753999999999998E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.6524000000000001E-3</v>
       </c>
       <c r="D20" s="17">
-        <f>D16</f>
-        <v>5.9068000000000002E-3</v>
+        <f t="shared" si="3"/>
+        <v>9.6270000000000001E-3</v>
       </c>
       <c r="E20" s="17">
-        <f t="shared" ref="E20:H20" si="3">E16</f>
-        <v>8.3766000000000014E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.56058E-2</v>
       </c>
       <c r="F20" s="17">
         <f t="shared" si="3"/>
-        <v>2.2221399999999999E-2</v>
+        <v>3.8330200000000002E-2</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" si="3"/>
-        <v>7.6724959999999995E-2</v>
+        <v>0.45484780000000002</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" si="3"/>
-        <v>0.52532100000000004</v>
+        <v>0.59586379999999994</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
@@ -10809,7 +10818,7 @@
     </row>
     <row r="22" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
@@ -10835,7 +10844,7 @@
     </row>
     <row r="23" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="21">
         <f>B19/B19</f>
@@ -10843,32 +10852,32 @@
       </c>
       <c r="C23" s="16">
         <f>B19/C19</f>
-        <v>0.22829581993569131</v>
+        <v>22.68147822261329</v>
       </c>
       <c r="D23" s="16">
         <f>B19/D19</f>
-        <v>8.8040782584734106E-2</v>
+        <v>10.065404139008201</v>
       </c>
       <c r="E23" s="16">
         <f>B19/E19</f>
-        <v>3.9920034984694201E-2</v>
+        <v>6.4661984196663731</v>
       </c>
       <c r="F23" s="21">
         <f>B19/F19</f>
-        <v>3.7570555032925688E-2</v>
+        <v>2.0492894762993146</v>
       </c>
       <c r="G23" s="16">
         <f>B19/G19</f>
-        <v>1.7310711835975725E-3</v>
+        <v>0.22473452947638234</v>
       </c>
       <c r="H23" s="16">
         <f>B19/H19</f>
-        <v>1.6275734891456897E-3</v>
+        <v>0.23465929909445316</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="22">
         <f>B20/B20</f>
@@ -10876,32 +10885,32 @@
       </c>
       <c r="C24" s="17">
         <f>B20/C20</f>
-        <v>0.24219435413118648</v>
+        <v>7.7422687707876294</v>
       </c>
       <c r="D24" s="17">
         <f>B20/D20</f>
-        <v>0.15890160492991129</v>
+        <v>4.5457982756829747</v>
       </c>
       <c r="E24" s="17">
         <f>B20/E20</f>
-        <v>0.11205023517895088</v>
+        <v>2.8042394494354665</v>
       </c>
       <c r="F24" s="17">
         <f>B20/F20</f>
-        <v>4.2238562826824595E-2</v>
+        <v>1.1417211493809059</v>
       </c>
       <c r="G24" s="17">
         <f>B20/G20</f>
-        <v>1.2233307127172176E-2</v>
+        <v>9.6213282772830824E-2</v>
       </c>
       <c r="H24" s="17">
         <f>B20/H20</f>
-        <v>1.7867170739414566E-3</v>
+        <v>7.3443629232049348E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -10919,7 +10928,7 @@
     </row>
     <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -10945,68 +10954,68 @@
     </row>
     <row r="28" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="21">
         <f t="shared" ref="B28:H29" si="4">1/B19</f>
-        <v>7824.7261345852885</v>
+        <v>48.491901852390647</v>
       </c>
       <c r="C28" s="16">
         <f t="shared" si="4"/>
-        <v>1786.3522686673809</v>
+        <v>1099.8680158380994</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" si="4"/>
-        <v>688.8950124001102</v>
+        <v>488.09058961343226</v>
       </c>
       <c r="E28" s="21">
         <f t="shared" si="4"/>
-        <v>312.36334103829574</v>
+        <v>313.55825912454526</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="4"/>
-        <v>293.97930385700846</v>
+        <v>99.373944151843389</v>
       </c>
       <c r="G28" s="16">
         <f t="shared" si="4"/>
-        <v>13.545157931123414</v>
+        <v>10.897804746211925</v>
       </c>
       <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>12.735316816476443</v>
+        <v>11.379075700439005</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="22">
         <f t="shared" si="4"/>
-        <v>1065.4165778819518</v>
+        <v>22.850666325430051</v>
       </c>
       <c r="C29" s="17">
         <f t="shared" si="4"/>
-        <v>258.03787996077824</v>
+        <v>176.91600028306559</v>
       </c>
       <c r="D29" s="17">
         <f t="shared" si="4"/>
-        <v>169.29640414437597</v>
+        <v>103.87451958034694</v>
       </c>
       <c r="E29" s="17">
         <f t="shared" si="4"/>
-        <v>119.38017811522573</v>
+        <v>64.078739955657511</v>
       </c>
       <c r="F29" s="17">
         <f t="shared" si="4"/>
-        <v>45.001665061607284</v>
+        <v>26.089089021189558</v>
       </c>
       <c r="G29" s="17">
         <f t="shared" si="4"/>
-        <v>13.03356821561067</v>
+        <v>2.1985376207162042</v>
       </c>
       <c r="H29" s="17">
         <f t="shared" si="4"/>
-        <v>1.9035979905619611</v>
+        <v>1.6782358653101599</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>